<commit_message>
:poop: Find station id by name
</commit_message>
<xml_diff>
--- a/assets/OutputData.xlsx
+++ b/assets/OutputData.xlsx
@@ -410,7 +410,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>idCommune</v>
+        <v>stationId</v>
       </c>
       <c r="B1" t="str">
         <v>date</v>
@@ -426,343 +426,343 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2">
+      <c r="A2" t="str">
         <v>79049004</v>
       </c>
       <c r="B2" t="str">
         <v>24/1/21 19:00</v>
       </c>
       <c r="D2" t="str">
-        <v>-4.7</v>
+        <v>-4,7</v>
       </c>
       <c r="E2" t="str">
-        <v>13.7</v>
+        <v>13,7</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3">
+      <c r="A3" t="str">
         <v>79049004</v>
       </c>
       <c r="B3" t="str">
         <v>25/1/21 8:23</v>
       </c>
       <c r="D3" t="str">
-        <v>0.6</v>
+        <v>0,6</v>
       </c>
       <c r="E3" t="str">
-        <v>4.7</v>
+        <v>4,7</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4">
+      <c r="A4" t="str">
         <v>79049004</v>
       </c>
       <c r="B4" t="str">
         <v>25/1/21 13:20</v>
       </c>
       <c r="D4" t="str">
-        <v>1.2</v>
+        <v>1,2</v>
       </c>
       <c r="E4" t="str">
-        <v>5.9</v>
+        <v>5,9</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5">
+      <c r="A5" t="str">
         <v>79049004</v>
       </c>
       <c r="B5" t="str">
         <v>25/1/21 19:20</v>
       </c>
       <c r="D5" t="str">
-        <v>-0.6</v>
+        <v>-0,6</v>
       </c>
       <c r="E5" t="str">
-        <v>6.3</v>
+        <v>6,3</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6">
+      <c r="A6" t="str">
         <v>79049004</v>
       </c>
       <c r="B6" t="str">
         <v>26/1/21 6:44</v>
       </c>
       <c r="D6" t="str">
-        <v>-4.8</v>
+        <v>-4,8</v>
       </c>
       <c r="E6" t="str">
-        <v>0.3</v>
+        <v>0,3</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7">
+      <c r="A7" t="str">
         <v>79049004</v>
       </c>
       <c r="B7" t="str">
         <v>26/1/21 13:29</v>
       </c>
       <c r="D7" t="str">
-        <v>-2.1</v>
+        <v>-2,1</v>
       </c>
       <c r="E7" t="str">
-        <v>3.3</v>
+        <v>3,3</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8">
+      <c r="A8" t="str">
         <v>79049004</v>
       </c>
       <c r="B8" t="str">
         <v>26/1/21 19:36</v>
       </c>
       <c r="D8" t="str">
-        <v>3.4</v>
+        <v>3,4</v>
       </c>
       <c r="E8" t="str">
-        <v>4.2</v>
+        <v>4,2</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9">
+      <c r="A9" t="str">
         <v>79049004</v>
       </c>
       <c r="B9" t="str">
         <v>27/1/21 6:30</v>
       </c>
       <c r="D9" t="str">
-        <v>2.3</v>
+        <v>2,3</v>
       </c>
       <c r="E9" t="str">
-        <v>4.8</v>
+        <v>4,8</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10">
+      <c r="A10" t="str">
         <v>79049004</v>
       </c>
       <c r="B10" t="str">
         <v>27/1/21 13:13</v>
       </c>
       <c r="D10" t="str">
-        <v>4.6</v>
+        <v>4,6</v>
       </c>
       <c r="E10" t="str">
-        <v>9.8</v>
+        <v>9,8</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11">
+      <c r="A11" t="str">
         <v>79049004</v>
       </c>
       <c r="B11" t="str">
         <v>27/1/21 20:01</v>
       </c>
       <c r="D11" t="str">
-        <v>9.8</v>
+        <v>9,8</v>
       </c>
       <c r="E11" t="str">
-        <v>10.6</v>
+        <v>10,6</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12">
+      <c r="A12" t="str">
         <v>79049004</v>
       </c>
       <c r="B12" t="str">
         <v>28/1/21 6:53</v>
       </c>
       <c r="D12" t="str">
-        <v>10.6</v>
+        <v>10,6</v>
       </c>
       <c r="E12" t="str">
-        <v>11.4</v>
+        <v>11,4</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13">
+      <c r="A13" t="str">
         <v>79049004</v>
       </c>
       <c r="B13" t="str">
         <v>28/1/21 13:25</v>
       </c>
       <c r="D13" t="str">
-        <v>11.3</v>
+        <v>11,3</v>
       </c>
       <c r="E13" t="str">
-        <v>12.2</v>
+        <v>12,2</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14">
+      <c r="A14" t="str">
         <v>79049004</v>
       </c>
       <c r="B14" t="str">
         <v>28/1/21 19:12</v>
       </c>
       <c r="D14" t="str">
-        <v>11.3</v>
+        <v>11,3</v>
       </c>
       <c r="E14" t="str">
-        <v>12.3</v>
+        <v>12,3</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15">
+      <c r="A15" t="str">
         <v>79049004</v>
       </c>
       <c r="B15" t="str">
         <v>29/1/21 6:52</v>
       </c>
       <c r="D15" t="str">
-        <v>10.2</v>
+        <v>10,2</v>
       </c>
       <c r="E15" t="str">
-        <v>11.7</v>
+        <v>11,7</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16">
+      <c r="A16" t="str">
         <v>79049004</v>
       </c>
       <c r="B16" t="str">
         <v>29/1/21 13:33</v>
       </c>
       <c r="D16" t="str">
-        <v>9.9</v>
+        <v>9,9</v>
       </c>
       <c r="E16" t="str">
-        <v>11.8</v>
+        <v>11,8</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17">
+      <c r="A17" t="str">
         <v>79049004</v>
       </c>
       <c r="B17" t="str">
         <v>29/1/21 21:07</v>
       </c>
       <c r="D17" t="str">
-        <v>9.5</v>
+        <v>9,5</v>
       </c>
       <c r="E17" t="str">
-        <v>12.3</v>
+        <v>12,3</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18">
+      <c r="A18" t="str">
         <v>79049004</v>
       </c>
       <c r="B18" t="str">
         <v>30/1/21 6:35</v>
       </c>
       <c r="D18" t="str">
-        <v>8.7</v>
+        <v>8,7</v>
       </c>
       <c r="E18" t="str">
-        <v>11.3</v>
+        <v>11,3</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19">
+      <c r="A19" t="str">
         <v>79049004</v>
       </c>
       <c r="B19" t="str">
         <v>30/1/21 15:22</v>
       </c>
       <c r="D19" t="str">
-        <v>9.7</v>
+        <v>9,7</v>
       </c>
       <c r="E19" t="str">
-        <v>11.1</v>
+        <v>11,1</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20">
+      <c r="A20" t="str">
         <v>79049004</v>
       </c>
       <c r="B20" t="str">
         <v>31/1/21 8:17</v>
       </c>
       <c r="D20" t="str">
-        <v>8.6</v>
+        <v>8,6</v>
       </c>
       <c r="E20" t="str">
-        <v>9.9</v>
+        <v>9,9</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21">
+      <c r="A21" t="str">
         <v>79049004</v>
       </c>
       <c r="B21" t="str">
         <v>31/1/21 10:56</v>
       </c>
       <c r="D21" t="str">
-        <v>8.7</v>
+        <v>8,7</v>
       </c>
       <c r="E21" t="str">
-        <v>9.5</v>
+        <v>9,5</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22">
+      <c r="A22" t="str">
         <v>79049004</v>
       </c>
       <c r="B22" t="str">
         <v>31/1/21 20:34</v>
       </c>
       <c r="D22" t="str">
-        <v>9.6</v>
+        <v>9,6</v>
       </c>
       <c r="E22" t="str">
-        <v>10.9</v>
+        <v>10,9</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23">
+      <c r="A23" t="str">
         <v>79049004</v>
       </c>
       <c r="B23" t="str">
         <v>1/2/21 7:40</v>
       </c>
       <c r="D23" t="str">
-        <v>9.6</v>
+        <v>9,6</v>
       </c>
       <c r="E23" t="str">
-        <v>10.1</v>
+        <v>10,1</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24">
+      <c r="A24" t="str">
         <v>79049004</v>
       </c>
       <c r="B24" t="str">
         <v>1/2/21 13:23</v>
       </c>
       <c r="D24" t="str">
-        <v>9.8</v>
+        <v>9,8</v>
       </c>
       <c r="E24" t="str">
-        <v>11.1</v>
+        <v>11,1</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25">
+      <c r="A25" t="str">
         <v>79049004</v>
       </c>
       <c r="B25" t="str">
         <v>1/2/21 20:20</v>
       </c>
       <c r="D25" t="str">
-        <v>9.5</v>
+        <v>9,5</v>
       </c>
       <c r="E25" t="str">
-        <v>11.1</v>
+        <v>11,1</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26">
+      <c r="A26" t="str">
         <v>79049004</v>
       </c>
       <c r="B26" t="str">
@@ -772,67 +772,67 @@
         <v>9</v>
       </c>
       <c r="E26" t="str">
-        <v>11.8</v>
+        <v>11,8</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27">
+      <c r="A27" t="str">
         <v>79049004</v>
       </c>
       <c r="B27" t="str">
         <v>2/2/21 13:38</v>
       </c>
       <c r="D27" t="str">
-        <v>11.7</v>
+        <v>11,7</v>
       </c>
       <c r="E27" t="str">
-        <v>12.9</v>
+        <v>12,9</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28">
+      <c r="A28" t="str">
         <v>79049004</v>
       </c>
       <c r="B28" t="str">
         <v>2/2/21 23:28</v>
       </c>
       <c r="D28" t="str">
-        <v>11.2</v>
+        <v>11,2</v>
       </c>
       <c r="E28" t="str">
         <v>13</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29">
+      <c r="A29" t="str">
         <v>79049004</v>
       </c>
       <c r="B29" t="str">
         <v>3/2/21 13:29</v>
       </c>
       <c r="D29" t="str">
-        <v>9.8</v>
+        <v>9,8</v>
       </c>
       <c r="E29" t="str">
-        <v>11.9</v>
+        <v>11,9</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30">
+      <c r="A30" t="str">
         <v>79049004</v>
       </c>
       <c r="B30" t="str">
         <v>3/2/21 22:37</v>
       </c>
       <c r="D30" t="str">
-        <v>7.7</v>
+        <v>7,7</v>
       </c>
       <c r="E30" t="str">
         <v>12</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31">
+      <c r="A31" t="str">
         <v>79049004</v>
       </c>
       <c r="B31" t="str">
@@ -842,46 +842,46 @@
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <v>8.7</v>
+        <v>8,7</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32">
+      <c r="A32" t="str">
         <v>79049004</v>
       </c>
       <c r="B32" t="str">
         <v>4/2/21 17:39</v>
       </c>
       <c r="D32" t="str">
-        <v>8.4</v>
+        <v>8,4</v>
       </c>
       <c r="E32" t="str">
-        <v>12.9</v>
+        <v>12,9</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33">
+      <c r="A33" t="str">
         <v>79049004</v>
       </c>
       <c r="B33" t="str">
         <v>5/2/21 8:49</v>
       </c>
       <c r="D33" t="str">
-        <v>6.9</v>
+        <v>6,9</v>
       </c>
       <c r="E33" t="str">
-        <v>10.7</v>
+        <v>10,7</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34">
+      <c r="A34" t="str">
         <v>79049004</v>
       </c>
       <c r="B34" t="str">
         <v>5/2/21 18:22</v>
       </c>
       <c r="D34" t="str">
-        <v>7.3</v>
+        <v>7,3</v>
       </c>
       <c r="E34" t="str">
         <v>11</v>

</xml_diff>

<commit_message>
:poop: Save with good number format ?
</commit_message>
<xml_diff>
--- a/assets/OutputData.xlsx
+++ b/assets/OutputData.xlsx
@@ -438,10 +438,10 @@
         <v>44220.791666666664</v>
       </c>
       <c r="D2" t="str">
-        <v>-4.7</v>
+        <v>-4,7</v>
       </c>
       <c r="E2" t="str">
-        <v>13.7</v>
+        <v>13,7</v>
       </c>
     </row>
     <row r="3">
@@ -455,10 +455,10 @@
         <v>44221.34930555556</v>
       </c>
       <c r="D3" t="str">
-        <v>0.6</v>
+        <v>0,6</v>
       </c>
       <c r="E3" t="str">
-        <v>4.7</v>
+        <v>4,7</v>
       </c>
     </row>
     <row r="4">
@@ -472,10 +472,10 @@
         <v>44221.555555555555</v>
       </c>
       <c r="D4" t="str">
-        <v>1.2</v>
+        <v>1,2</v>
       </c>
       <c r="E4" t="str">
-        <v>5.9</v>
+        <v>5,9</v>
       </c>
     </row>
     <row r="5">
@@ -489,10 +489,10 @@
         <v>44221.805555555555</v>
       </c>
       <c r="D5" t="str">
-        <v>-0.6</v>
+        <v>-0,6</v>
       </c>
       <c r="E5" t="str">
-        <v>6.3</v>
+        <v>6,3</v>
       </c>
     </row>
     <row r="6">
@@ -506,10 +506,10 @@
         <v>44222.28055555555</v>
       </c>
       <c r="D6" t="str">
-        <v>-4.8</v>
+        <v>-4,8</v>
       </c>
       <c r="E6" t="str">
-        <v>0.3</v>
+        <v>0,3</v>
       </c>
     </row>
     <row r="7">
@@ -523,10 +523,10 @@
         <v>44222.56180555555</v>
       </c>
       <c r="D7" t="str">
-        <v>-2.1</v>
+        <v>-2,1</v>
       </c>
       <c r="E7" t="str">
-        <v>3.3</v>
+        <v>3,3</v>
       </c>
     </row>
     <row r="8">
@@ -540,10 +540,10 @@
         <v>44222.816666666666</v>
       </c>
       <c r="D8" t="str">
-        <v>3.4</v>
+        <v>3,4</v>
       </c>
       <c r="E8" t="str">
-        <v>4.2</v>
+        <v>4,2</v>
       </c>
     </row>
     <row r="9">
@@ -557,10 +557,10 @@
         <v>44223.270833333336</v>
       </c>
       <c r="D9" t="str">
-        <v>2.3</v>
+        <v>2,3</v>
       </c>
       <c r="E9" t="str">
-        <v>4.8</v>
+        <v>4,8</v>
       </c>
     </row>
     <row r="10">
@@ -574,10 +574,10 @@
         <v>44223.55069444444</v>
       </c>
       <c r="D10" t="str">
-        <v>4.6</v>
+        <v>4,6</v>
       </c>
       <c r="E10" t="str">
-        <v>9.8</v>
+        <v>9,8</v>
       </c>
     </row>
     <row r="11">
@@ -591,10 +591,10 @@
         <v>44223.834027777775</v>
       </c>
       <c r="D11" t="str">
-        <v>9.8</v>
+        <v>9,8</v>
       </c>
       <c r="E11" t="str">
-        <v>10.6</v>
+        <v>10,6</v>
       </c>
     </row>
     <row r="12">
@@ -608,10 +608,10 @@
         <v>44224.28680555556</v>
       </c>
       <c r="D12" t="str">
-        <v>10.6</v>
+        <v>10,6</v>
       </c>
       <c r="E12" t="str">
-        <v>11.4</v>
+        <v>11,4</v>
       </c>
     </row>
     <row r="13">
@@ -625,10 +625,10 @@
         <v>44224.55902777778</v>
       </c>
       <c r="D13" t="str">
-        <v>11.3</v>
+        <v>11,3</v>
       </c>
       <c r="E13" t="str">
-        <v>12.2</v>
+        <v>12,2</v>
       </c>
     </row>
     <row r="14">
@@ -642,10 +642,10 @@
         <v>44224.8</v>
       </c>
       <c r="D14" t="str">
-        <v>11.3</v>
+        <v>11,3</v>
       </c>
       <c r="E14" t="str">
-        <v>12.3</v>
+        <v>12,3</v>
       </c>
     </row>
     <row r="15">
@@ -659,10 +659,10 @@
         <v>44225.28611111111</v>
       </c>
       <c r="D15" t="str">
-        <v>10.2</v>
+        <v>10,2</v>
       </c>
       <c r="E15" t="str">
-        <v>11.7</v>
+        <v>11,7</v>
       </c>
     </row>
     <row r="16">
@@ -676,10 +676,10 @@
         <v>44225.56458333333</v>
       </c>
       <c r="D16" t="str">
-        <v>9.9</v>
+        <v>9,9</v>
       </c>
       <c r="E16" t="str">
-        <v>11.8</v>
+        <v>11,8</v>
       </c>
     </row>
     <row r="17">
@@ -693,10 +693,10 @@
         <v>44225.87986111111</v>
       </c>
       <c r="D17" t="str">
-        <v>9.5</v>
+        <v>9,5</v>
       </c>
       <c r="E17" t="str">
-        <v>12.3</v>
+        <v>12,3</v>
       </c>
     </row>
     <row r="18">
@@ -710,10 +710,10 @@
         <v>44226.274305555555</v>
       </c>
       <c r="D18" t="str">
-        <v>8.7</v>
+        <v>8,7</v>
       </c>
       <c r="E18" t="str">
-        <v>11.3</v>
+        <v>11,3</v>
       </c>
     </row>
     <row r="19">
@@ -727,10 +727,10 @@
         <v>44226.64027777778</v>
       </c>
       <c r="D19" t="str">
-        <v>9.7</v>
+        <v>9,7</v>
       </c>
       <c r="E19" t="str">
-        <v>11.1</v>
+        <v>11,1</v>
       </c>
     </row>
     <row r="20">
@@ -744,10 +744,10 @@
         <v>44227.345138888886</v>
       </c>
       <c r="D20" t="str">
-        <v>8.6</v>
+        <v>8,6</v>
       </c>
       <c r="E20" t="str">
-        <v>9.9</v>
+        <v>9,9</v>
       </c>
     </row>
     <row r="21">
@@ -761,10 +761,10 @@
         <v>44227.455555555556</v>
       </c>
       <c r="D21" t="str">
-        <v>8.7</v>
+        <v>8,7</v>
       </c>
       <c r="E21" t="str">
-        <v>9.5</v>
+        <v>9,5</v>
       </c>
     </row>
     <row r="22">
@@ -778,10 +778,10 @@
         <v>44227.856944444444</v>
       </c>
       <c r="D22" t="str">
-        <v>9.6</v>
+        <v>9,6</v>
       </c>
       <c r="E22" t="str">
-        <v>10.9</v>
+        <v>10,9</v>
       </c>
     </row>
     <row r="23">
@@ -795,10 +795,10 @@
         <v>44228.319444444445</v>
       </c>
       <c r="D23" t="str">
-        <v>9.6</v>
+        <v>9,6</v>
       </c>
       <c r="E23" t="str">
-        <v>10.1</v>
+        <v>10,1</v>
       </c>
     </row>
     <row r="24">
@@ -812,10 +812,10 @@
         <v>44228.55763888889</v>
       </c>
       <c r="D24" t="str">
-        <v>9.8</v>
+        <v>9,8</v>
       </c>
       <c r="E24" t="str">
-        <v>11.1</v>
+        <v>11,1</v>
       </c>
     </row>
     <row r="25">
@@ -829,10 +829,10 @@
         <v>44228.84722222222</v>
       </c>
       <c r="D25" t="str">
-        <v>9.5</v>
+        <v>9,5</v>
       </c>
       <c r="E25" t="str">
-        <v>11.1</v>
+        <v>11,1</v>
       </c>
     </row>
     <row r="26">
@@ -849,7 +849,7 @@
         <v>9</v>
       </c>
       <c r="E26" t="str">
-        <v>11.8</v>
+        <v>11,8</v>
       </c>
     </row>
     <row r="27">
@@ -863,10 +863,10 @@
         <v>44229.56805555556</v>
       </c>
       <c r="D27" t="str">
-        <v>11.7</v>
+        <v>11,7</v>
       </c>
       <c r="E27" t="str">
-        <v>12.9</v>
+        <v>12,9</v>
       </c>
     </row>
     <row r="28">
@@ -880,7 +880,7 @@
         <v>44229.97777777778</v>
       </c>
       <c r="D28" t="str">
-        <v>11.2</v>
+        <v>11,2</v>
       </c>
       <c r="E28" t="str">
         <v>13</v>
@@ -897,10 +897,10 @@
         <v>44230.56180555555</v>
       </c>
       <c r="D29" t="str">
-        <v>9.8</v>
+        <v>9,8</v>
       </c>
       <c r="E29" t="str">
-        <v>11.9</v>
+        <v>11,9</v>
       </c>
     </row>
     <row r="30">
@@ -914,7 +914,7 @@
         <v>44230.94236111111</v>
       </c>
       <c r="D30" t="str">
-        <v>7.7</v>
+        <v>7,7</v>
       </c>
       <c r="E30" t="str">
         <v>12</v>
@@ -934,7 +934,7 @@
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <v>8.7</v>
+        <v>8,7</v>
       </c>
     </row>
     <row r="32">
@@ -948,10 +948,10 @@
         <v>44231.73541666667</v>
       </c>
       <c r="D32" t="str">
-        <v>8.4</v>
+        <v>8,4</v>
       </c>
       <c r="E32" t="str">
-        <v>12.9</v>
+        <v>12,9</v>
       </c>
     </row>
     <row r="33">
@@ -965,10 +965,10 @@
         <v>44232.36736111111</v>
       </c>
       <c r="D33" t="str">
-        <v>6.9</v>
+        <v>6,9</v>
       </c>
       <c r="E33" t="str">
-        <v>10.7</v>
+        <v>10,7</v>
       </c>
     </row>
     <row r="34">
@@ -982,7 +982,7 @@
         <v>44232.76527777778</v>
       </c>
       <c r="D34" t="str">
-        <v>7.3</v>
+        <v>7,3</v>
       </c>
       <c r="E34" t="str">
         <v>11</v>
@@ -999,10 +999,10 @@
         <v>44909.32152777778</v>
       </c>
       <c r="D35" t="str">
-        <v>-5.2</v>
+        <v>-5,2</v>
       </c>
       <c r="E35" t="str">
-        <v>40.4</v>
+        <v>40,4</v>
       </c>
     </row>
     <row r="36">
@@ -1016,10 +1016,10 @@
         <v>44910.34097222222</v>
       </c>
       <c r="D36" t="str">
-        <v>0.7</v>
+        <v>0,7</v>
       </c>
       <c r="E36" t="str">
-        <v>7.9</v>
+        <v>7,9</v>
       </c>
     </row>
     <row r="37">
@@ -1036,7 +1036,7 @@
         <v>-2</v>
       </c>
       <c r="E37" t="str">
-        <v>2.9</v>
+        <v>2,9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>